<commit_message>
Update log book & burndown chart + Tambah gambar slide cara kerja
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -658,7 +658,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -686,11 +686,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="67467136"/>
-        <c:axId val="67468672"/>
+        <c:axId val="61310464"/>
+        <c:axId val="61312000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67467136"/>
+        <c:axId val="61310464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,14 +753,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67468672"/>
+        <c:crossAx val="61312000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67468672"/>
+        <c:axId val="61312000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67467136"/>
+        <c:crossAx val="61310464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -909,7 +909,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1794,7 +1794,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1804,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1915,7 +1915,9 @@
       <c r="J5" s="3">
         <v>0</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -1951,7 +1953,9 @@
       <c r="J6" s="3">
         <v>0</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -1987,7 +1991,9 @@
       <c r="J7" s="3">
         <v>2</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -2023,7 +2029,9 @@
       <c r="J8" s="3">
         <v>0</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -2059,7 +2067,9 @@
       <c r="J9" s="3">
         <v>1</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -2095,7 +2105,9 @@
       <c r="J10" s="3">
         <v>1</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -2131,7 +2143,9 @@
       <c r="J11" s="3">
         <v>6</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3">
+        <v>5</v>
+      </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -2167,7 +2181,9 @@
       <c r="J12" s="3">
         <v>4</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="3">
+        <v>4</v>
+      </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -2203,7 +2219,9 @@
       <c r="J13" s="3">
         <v>2</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -2239,7 +2257,9 @@
       <c r="J14" s="3">
         <v>5</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="3">
+        <v>5</v>
+      </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -2338,7 +2358,7 @@
       </c>
       <c r="K16" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Update Log Book dan Burndown Chart
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester 4\TKPPL\ProjekTKPPL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10965" windowHeight="5010"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +30,7 @@
     <author>mkg</author>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,8 +160,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,7 +290,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -318,6 +333,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -325,11 +341,37 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -389,7 +431,13 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -505,6 +553,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -565,7 +614,13 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -661,13 +716,13 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -681,19 +736,26 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:axId val="61310464"/>
-        <c:axId val="61312000"/>
+        <c:smooth val="0"/>
+        <c:axId val="421281776"/>
+        <c:axId val="421277424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61310464"/>
+        <c:axId val="421281776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -721,6 +783,8 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -753,17 +817,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61312000"/>
+        <c:crossAx val="421277424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61312000"/>
+        <c:axId val="421277424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -791,6 +857,8 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -823,7 +891,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61310464"/>
+        <c:crossAx val="421281776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -838,6 +906,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -872,6 +941,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1794,28 +1864,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" customHeight="1">
+    <row r="1" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1827,7 +1897,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="2:17" ht="15" customHeight="1">
+    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1837,7 +1907,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="4" spans="2:17">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1887,7 +1957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:17">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1918,14 +1988,20 @@
       <c r="K5" s="3">
         <v>0</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="2:17">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1956,14 +2032,20 @@
       <c r="K6" s="3">
         <v>0</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="2:17">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1994,14 +2076,20 @@
       <c r="K7" s="3">
         <v>1</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="2:17">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2032,14 +2120,20 @@
       <c r="K8" s="3">
         <v>0</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="2:17">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
@@ -2070,14 +2164,20 @@
       <c r="K9" s="3">
         <v>0</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="2:17">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2108,14 +2208,20 @@
       <c r="K10" s="3">
         <v>0</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="2:17">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -2146,14 +2252,20 @@
       <c r="K11" s="3">
         <v>5</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="L11" s="3">
+        <v>3</v>
+      </c>
+      <c r="M11" s="3">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="2:17">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
@@ -2184,14 +2296,20 @@
       <c r="K12" s="3">
         <v>4</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="L12" s="3">
+        <v>4</v>
+      </c>
+      <c r="M12" s="3">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="2:17">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2222,14 +2340,20 @@
       <c r="K13" s="3">
         <v>2</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="L13" s="3">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>2</v>
+      </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="2:17">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
@@ -2260,14 +2384,20 @@
       <c r="K14" s="3">
         <v>5</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="L14" s="3">
+        <v>5</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5</v>
+      </c>
+      <c r="N14" s="3">
+        <v>4</v>
+      </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="2:17">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2326,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>18</v>
       </c>
@@ -2362,15 +2492,15 @@
       </c>
       <c r="L16" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="2"/>
@@ -2402,12 +2532,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edit Back Log dan Isi Burndown Chart
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester 4\TKPPL\ProjekTKPPL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10965" windowHeight="5010"/>
   </bookViews>
@@ -15,49 +10,16 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>mkg</author>
-  </authors>
-  <commentList>
-    <comment ref="F4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>goodoldmanoj.com:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Remaining effort as of that day to complete the task. NOT last day effort - hours worked. So this can go up if new challenges got uncovered</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
@@ -160,8 +122,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,19 +135,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -250,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -268,8 +217,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -290,17 +242,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -333,7 +275,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -341,37 +282,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -431,13 +346,7 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -553,7 +462,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -614,13 +522,7 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -725,7 +627,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -736,26 +638,19 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="421281776"/>
-        <c:axId val="421277424"/>
+        <c:marker val="1"/>
+        <c:axId val="61160448"/>
+        <c:axId val="61174528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421281776"/>
+        <c:axId val="61160448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -783,8 +678,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -817,19 +710,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421277424"/>
+        <c:crossAx val="61174528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421277424"/>
+        <c:axId val="61174528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -857,8 +748,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -891,7 +780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421281776"/>
+        <c:crossAx val="61160448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -906,7 +795,6 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -941,7 +829,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -979,599 +866,10 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1864,28 +1162,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" ht="15" customHeight="1">
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1195,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" ht="15" customHeight="1">
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1907,7 +1205,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1947,17 +1245,17 @@
       <c r="N4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1997,11 +1295,13 @@
       <c r="N5" s="3">
         <v>0</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2041,11 +1341,13 @@
       <c r="N6" s="3">
         <v>0</v>
       </c>
-      <c r="O6" s="3"/>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2085,11 +1387,13 @@
       <c r="N7" s="3">
         <v>0</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2129,11 +1433,13 @@
       <c r="N8" s="3">
         <v>0</v>
       </c>
-      <c r="O8" s="3"/>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
@@ -2173,11 +1479,13 @@
       <c r="N9" s="3">
         <v>0</v>
       </c>
-      <c r="O9" s="3"/>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2217,11 +1525,13 @@
       <c r="N10" s="3">
         <v>0</v>
       </c>
-      <c r="O10" s="3"/>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -2261,11 +1571,13 @@
       <c r="N11" s="3">
         <v>0</v>
       </c>
-      <c r="O11" s="3"/>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17">
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
@@ -2305,11 +1617,13 @@
       <c r="N12" s="3">
         <v>0</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17">
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2349,11 +1663,13 @@
       <c r="N13" s="3">
         <v>2</v>
       </c>
-      <c r="O13" s="3"/>
+      <c r="O13" s="3">
+        <v>2</v>
+      </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17">
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
@@ -2393,11 +1709,13 @@
       <c r="N14" s="3">
         <v>4</v>
       </c>
-      <c r="O14" s="3"/>
+      <c r="O14" s="3">
+        <v>4</v>
+      </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17">
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2456,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17">
       <c r="B16" s="5" t="s">
         <v>18</v>
       </c>
@@ -2504,7 +1822,7 @@
       </c>
       <c r="O16" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P16" s="3">
         <f t="shared" si="2"/>
@@ -2524,20 +1842,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="E15:F15 E16 F16:H16 G15:K15 I16:J16 L15:Q15 K16:Q16" unlockedFormula="1"/>
+    <ignoredError sqref="E15:F15 E16 F16:H16 G15:K15 I16:J16 L15:N15 K16:Q16 P15:Q15" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>